<commit_message>
Updated to include some report fixes and an option to skip phones
</commit_message>
<xml_diff>
--- a/nda-config.xlsx
+++ b/nda-config.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Variable</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>192.168.0.0/16,10.0.0.0/8,172.16.0.0/12</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryIncludePhones</t>
+  </si>
+  <si>
+    <t>Remove phones from CDP/LLDP discovery (Cisco Only)</t>
   </si>
 </sst>
 </file>
@@ -517,20 +523,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="140.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.41796875" customWidth="1"/>
+    <col min="2" max="2" width="27.68359375" customWidth="1"/>
+    <col min="3" max="3" width="140.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -552,7 +558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -563,7 +569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -572,7 +578,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -581,7 +587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -592,7 +598,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -601,7 +607,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -610,7 +616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -621,91 +627,102 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="6" t="b">
+      <c r="B11" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
       </c>
       <c r="B14" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B16" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>20</v>
       </c>
     </row>
@@ -723,18 +740,18 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.83984375" customWidth="1"/>
+    <col min="2" max="2" width="24.578125" customWidth="1"/>
+    <col min="3" max="3" width="32.26171875" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.83984375" customWidth="1"/>
+    <col min="6" max="6" width="8.68359375" customWidth="1"/>
+    <col min="7" max="7" width="8.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -762,14 +779,14 @@
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.15625" customWidth="1"/>
+    <col min="2" max="2" width="33.41796875" customWidth="1"/>
+    <col min="3" max="3" width="36.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -794,13 +811,13 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.15625" customWidth="1"/>
+    <col min="2" max="2" width="7.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -808,7 +825,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Major module update, moving code to module based design
Dev branch is nda-test.py
</commit_message>
<xml_diff>
--- a/nda-config.xlsx
+++ b/nda-config.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Variable</t>
   </si>
@@ -35,145 +35,169 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ExportLocation</t>
+  </si>
+  <si>
+    <t>Specify the output folder</t>
+  </si>
+  <si>
+    <t>Specify True/False for whether you want to just gather data and not do any reachability tests</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Device IPs</t>
+  </si>
+  <si>
+    <t>HealthCheck</t>
+  </si>
+  <si>
+    <t>Specify True/False for whether you want to check health</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Specify the IP of a seed router</t>
+  </si>
+  <si>
+    <t>C:\test</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryDomains</t>
+  </si>
+  <si>
+    <t>Comma separated list of domains you want to truncate from hostnames</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryExcludedSubnets</t>
+  </si>
+  <si>
+    <t>Comma separated list of subnets you want to exclude from discovery</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryIncludedSubnets</t>
+  </si>
+  <si>
+    <t>Comma separated list of subnets you want to include into discovery</t>
+  </si>
+  <si>
+    <t>Specify True/False for whether you want to do a slower SSH CDP crawl of all devices (still will attempt the SNMP method)</t>
+  </si>
+  <si>
+    <t>Specify True/False for whether you want to do CDP discovery of devices (SNMP method)</t>
+  </si>
+  <si>
+    <t>DeviceDiscovery</t>
+  </si>
+  <si>
+    <t>DeviceDiscoverySSH</t>
+  </si>
+  <si>
+    <t>DeviceDiscoverySeed</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryDepth</t>
+  </si>
+  <si>
+    <t>DeviceDiscoverySSHType</t>
+  </si>
+  <si>
+    <t>(IOS/XE/NXOS) Specify the type of device if you are doing a manual SSH method</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryMap</t>
+  </si>
+  <si>
+    <t>Create topology map of enviroment</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryMapTitle</t>
+  </si>
+  <si>
+    <t>Network Topology</t>
+  </si>
+  <si>
+    <t>Create a name for the map</t>
+  </si>
+  <si>
+    <t>(0 means no limit) Specify an integer for how deep you want to discover devices</t>
+  </si>
+  <si>
+    <t>SNMP Community</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Enable Password</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>192.168.0.0/16,10.0.0.0/8,172.16.0.0/12</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryIncludePhones</t>
+  </si>
+  <si>
+    <t>Remove phones from CDP/LLDP discovery (Cisco Only)</t>
+  </si>
+  <si>
+    <t>Specify True/False, this will create a full inventory report</t>
+  </si>
+  <si>
+    <t>Specify True/False, this will create a ARP/MAC report (this is time consuming)</t>
+  </si>
+  <si>
+    <t>Specify True/False, this will create a POE report</t>
+  </si>
+  <si>
+    <t>FullInventoryReport</t>
+  </si>
+  <si>
+    <t>ARPMACReport</t>
+  </si>
+  <si>
+    <t>POEReport</t>
+  </si>
+  <si>
+    <t>InterfaceReport</t>
+  </si>
+  <si>
+    <t>Specify True/False, this will create a interface report</t>
+  </si>
+  <si>
     <t>PowerBudget</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>ExportLocation</t>
-  </si>
-  <si>
-    <t>Specify the output folder</t>
+    <t>DHCPSnooping</t>
   </si>
   <si>
     <t>Temperature</t>
   </si>
   <si>
-    <t>DHCPSnooping</t>
-  </si>
-  <si>
-    <t>Specify True/False for whether you want to just gather data and not do any reachability tests</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Device IPs</t>
-  </si>
-  <si>
-    <t>HealthCheck</t>
-  </si>
-  <si>
-    <t>Specify True/False for whether you want to check health</t>
-  </si>
-  <si>
-    <t>Configuration</t>
-  </si>
-  <si>
-    <t>Specify the IP of a seed router</t>
-  </si>
-  <si>
-    <t>C:\test</t>
-  </si>
-  <si>
-    <t>Specify True/False, this will record the results of the power budget and export it with the final dump</t>
-  </si>
-  <si>
-    <t>Specify True/False, this will record the enviromental result and export it with the final dump</t>
-  </si>
-  <si>
-    <t>Specify True/False, this will validate DHCP Snooping is enabled and export results with the final dump</t>
-  </si>
-  <si>
-    <t>DeviceDiscoveryDomains</t>
-  </si>
-  <si>
-    <t>Comma separated list of domains you want to truncate from hostnames</t>
-  </si>
-  <si>
-    <t>DeviceDiscoveryExcludedSubnets</t>
-  </si>
-  <si>
-    <t>Comma separated list of subnets you want to exclude from discovery</t>
-  </si>
-  <si>
-    <t>DeviceDiscoveryIncludedSubnets</t>
-  </si>
-  <si>
-    <t>Comma separated list of subnets you want to include into discovery</t>
-  </si>
-  <si>
-    <t>Specify True/False for whether you want to do a slower SSH CDP crawl of all devices (still will attempt the SNMP method)</t>
-  </si>
-  <si>
-    <t>Specify True/False for whether you want to do CDP discovery of devices (SNMP method)</t>
-  </si>
-  <si>
-    <t>DeviceDiscovery</t>
-  </si>
-  <si>
-    <t>DeviceDiscoverySSH</t>
-  </si>
-  <si>
-    <t>DeviceDiscoverySeed</t>
-  </si>
-  <si>
-    <t>DeviceDiscoveryDepth</t>
-  </si>
-  <si>
-    <t>DeviceDiscoverySSHType</t>
-  </si>
-  <si>
-    <t>(IOS/XE/NXOS) Specify the type of device if you are doing a manual SSH method</t>
-  </si>
-  <si>
-    <t>DeviceDiscoveryMap</t>
-  </si>
-  <si>
-    <t>Create topology map of enviroment</t>
-  </si>
-  <si>
-    <t>DeviceDiscoveryMapTitle</t>
-  </si>
-  <si>
-    <t>Network Topology</t>
-  </si>
-  <si>
-    <t>Create a name for the map</t>
-  </si>
-  <si>
-    <t>(0 means no limit) Specify an integer for how deep you want to discover devices</t>
-  </si>
-  <si>
-    <t>SNMP Community</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Enable Password</t>
-  </si>
-  <si>
-    <t>public</t>
-  </si>
-  <si>
-    <t>192.168.0.0/16,10.0.0.0/8,172.16.0.0/12</t>
-  </si>
-  <si>
-    <t>DeviceDiscoveryIncludePhones</t>
-  </si>
-  <si>
-    <t>Remove phones from CDP/LLDP discovery (Cisco Only)</t>
+    <t>(Retiring) Specify True/False, this will record the results of the power budget and export it with the final dump</t>
+  </si>
+  <si>
+    <t>(Retiring) Specify True/False, this will record the enviromental result and export it with the final dump</t>
+  </si>
+  <si>
+    <t>(Retiring) Specify True/False, this will validate DHCP Snooping is enabled and export results with the final dump</t>
   </si>
 </sst>
 </file>
@@ -523,20 +547,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.41796875" customWidth="1"/>
-    <col min="2" max="2" width="27.68359375" customWidth="1"/>
-    <col min="3" max="3" width="140.83984375" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="140.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,186 +568,230 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5">
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B10" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
+      <c r="B19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -740,29 +808,29 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.83984375" customWidth="1"/>
-    <col min="2" max="2" width="24.578125" customWidth="1"/>
-    <col min="3" max="3" width="32.26171875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="7.83984375" customWidth="1"/>
-    <col min="6" max="6" width="8.68359375" customWidth="1"/>
-    <col min="7" max="7" width="8.26171875" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -779,22 +847,22 @@
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.15625" customWidth="1"/>
-    <col min="2" max="2" width="33.41796875" customWidth="1"/>
-    <col min="3" max="3" width="36.15625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -811,23 +879,23 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.15625" customWidth="1"/>
-    <col min="2" max="2" width="7.83984375" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>2</v>

</xml_diff>

<commit_message>
Updated XLSX to 0.6.1
Removed extra lines
</commit_message>
<xml_diff>
--- a/nda-config.xlsx
+++ b/nda-config.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Variable</t>
   </si>
@@ -180,24 +180,6 @@
   </si>
   <si>
     <t>Specify True/False, this will create a interface report</t>
-  </si>
-  <si>
-    <t>PowerBudget</t>
-  </si>
-  <si>
-    <t>DHCPSnooping</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>(Retiring) Specify True/False, this will record the results of the power budget and export it with the final dump</t>
-  </si>
-  <si>
-    <t>(Retiring) Specify True/False, this will record the enviromental result and export it with the final dump</t>
-  </si>
-  <si>
-    <t>(Retiring) Specify True/False, this will validate DHCP Snooping is enabled and export results with the final dump</t>
   </si>
 </sst>
 </file>
@@ -549,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,37 +744,13 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>54</v>
-      </c>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>56</v>
-      </c>
+      <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
-      </c>
+      <c r="B22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated CDP method to attempt to find other paths (based on CDP data)
Updated IOS CDP template
Added Phone include / AP include options
</commit_message>
<xml_diff>
--- a/nda-config.xlsx
+++ b/nda-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Dropbox\Heartland\Scripts\Network-Documentation-Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Username" sheetId="6" r:id="rId3"/>
     <sheet name="SNMP" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Variable</t>
   </si>
@@ -155,9 +155,6 @@
     <t>DeviceDiscoveryIncludePhones</t>
   </si>
   <si>
-    <t>Remove phones from CDP/LLDP discovery (Cisco Only)</t>
-  </si>
-  <si>
     <t>Specify True/False, this will create a full inventory report</t>
   </si>
   <si>
@@ -180,6 +177,15 @@
   </si>
   <si>
     <t>Specify True/False, this will create a interface report</t>
+  </si>
+  <si>
+    <t>DeviceDiscoveryIncludeAPs</t>
+  </si>
+  <si>
+    <t>Add APs from CDP/LLDP discovery (SSH Only)</t>
+  </si>
+  <si>
+    <t>Add phones from CDP/LLDP discovery (SNMP/SSH)</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:C23"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,116 +647,127 @@
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="6" t="b">
+        <v>50</v>
+      </c>
+      <c r="B11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7" t="b">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B16" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B17" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed some minor new clean install bugs
</commit_message>
<xml_diff>
--- a/nda-config.xlsx
+++ b/nda-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Dropbox\Heartland\Scripts\Network-Documentation-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -575,7 +575,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>

</xml_diff>